<commit_message>
Updated Gannt to 10/5 ...  We're behind on Ordering CPU and drafting CAD of robot...  But we are ahead on chasis construction (Thanks Stephan)
</commit_message>
<xml_diff>
--- a/Fieldroid_Gantt.xlsx
+++ b/Fieldroid_Gantt.xlsx
@@ -580,9 +580,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -616,9 +613,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="7" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -633,6 +627,12 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2285,7 +2285,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="2"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="14"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2572,10 +2572,10 @@
   </sheetPr>
   <dimension ref="A1:DE33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="9" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="B13" sqref="B13"/>
+      <selection pane="topRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2595,51 +2595,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:109" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="1:109" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="29" t="s">
         <v>9</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
-      <c r="O2" s="32">
-        <v>2</v>
+      <c r="O2" s="30">
+        <v>14</v>
       </c>
       <c r="P2" s="7"/>
       <c r="R2" s="9"/>
-      <c r="S2" s="33" t="s">
+      <c r="S2" s="31" t="s">
         <v>0</v>
       </c>
       <c r="U2" s="12"/>
-      <c r="V2" s="33" t="s">
+      <c r="V2" s="31" t="s">
         <v>1</v>
       </c>
       <c r="Y2" s="11"/>
-      <c r="Z2" s="34" t="s">
+      <c r="Z2" s="32" t="s">
         <v>39</v>
       </c>
       <c r="AD2" s="13"/>
-      <c r="AE2" s="34" t="s">
+      <c r="AE2" s="32" t="s">
         <v>40</v>
       </c>
       <c r="AH2" s="1"/>
@@ -2647,30 +2647,30 @@
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="10"/>
-      <c r="AM2" s="34" t="s">
+      <c r="AM2" s="32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:109" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:109" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="23" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="18" t="s">
         <v>43</v>
       </c>
       <c r="M3" s="15"/>
@@ -2679,7 +2679,7 @@
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
-      <c r="S3" s="19" t="s">
+      <c r="S3" s="18" t="s">
         <v>44</v>
       </c>
       <c r="U3" s="15"/>
@@ -2691,13 +2691,13 @@
       <c r="AA3" s="15"/>
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
-      <c r="AX3" s="20" t="s">
+      <c r="AX3" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="CB3" s="20" t="s">
+      <c r="CB3" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="CO3" s="20" t="s">
+      <c r="CO3" s="19" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2706,19 +2706,19 @@
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -2971,7 +2971,7 @@
       <c r="CM4" s="17">
         <v>12</v>
       </c>
-      <c r="CN4" s="29" t="s">
+      <c r="CN4" s="28" t="s">
         <v>38</v>
       </c>
       <c r="CO4" s="17">
@@ -3029,14 +3029,14 @@
     <row r="5" spans="1:109" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="18" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="18"/>
+      <c r="I5" s="34"/>
       <c r="J5" s="3">
         <v>1</v>
       </c>
@@ -3339,589 +3339,589 @@
       </c>
     </row>
     <row r="6" spans="1:109" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="26">
+      <c r="C6" s="20"/>
+      <c r="D6" s="25">
         <v>1</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="25">
         <v>5</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="25">
         <v>1</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="25">
         <v>5</v>
       </c>
-      <c r="H6" s="27">
-        <v>0.7</v>
+      <c r="H6" s="26">
+        <v>0.99</v>
       </c>
     </row>
     <row r="7" spans="1:109" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="26">
+      <c r="C7" s="20"/>
+      <c r="D7" s="25">
         <v>1</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="25">
         <v>10</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="25">
         <v>3</v>
       </c>
-      <c r="G7" s="26">
-        <v>8</v>
-      </c>
-      <c r="H7" s="27">
-        <v>0</v>
+      <c r="G7" s="25">
+        <v>10</v>
+      </c>
+      <c r="H7" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:109" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="26">
+      <c r="C8" s="20"/>
+      <c r="D8" s="25">
         <v>2</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="25">
         <v>9</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="25">
         <v>4</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="25">
         <v>7</v>
       </c>
-      <c r="H8" s="27">
-        <v>0</v>
+      <c r="H8" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:109" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="26">
+      <c r="C9" s="20"/>
+      <c r="D9" s="25">
         <v>3</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="25">
         <v>8</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="25">
         <v>4</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="25">
         <v>7</v>
       </c>
-      <c r="H9" s="27">
-        <v>0</v>
+      <c r="H9" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:109" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="26">
+      <c r="C10" s="20"/>
+      <c r="D10" s="25">
         <v>4</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="25">
         <v>7</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="25">
         <v>5</v>
       </c>
-      <c r="G10" s="26">
-        <v>6</v>
-      </c>
-      <c r="H10" s="27">
-        <v>0</v>
+      <c r="G10" s="25">
+        <v>11</v>
+      </c>
+      <c r="H10" s="26">
+        <v>0.8</v>
       </c>
     </row>
     <row r="11" spans="1:109" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="26">
+      <c r="C11" s="20"/>
+      <c r="D11" s="25">
         <v>3</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="25">
         <v>10</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="25">
         <v>7</v>
       </c>
-      <c r="G11" s="26">
-        <v>1</v>
-      </c>
-      <c r="H11" s="27">
-        <v>0</v>
+      <c r="G11" s="25">
+        <v>10</v>
+      </c>
+      <c r="H11" s="26">
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:109" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="8"/>
-      <c r="D12" s="26">
+      <c r="D12" s="25">
         <v>9</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="25">
         <v>8</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="25">
         <v>9</v>
       </c>
-      <c r="G12" s="26">
-        <v>1</v>
-      </c>
-      <c r="H12" s="27">
-        <v>0</v>
+      <c r="G12" s="25">
+        <v>8</v>
+      </c>
+      <c r="H12" s="26">
+        <v>0.8</v>
       </c>
     </row>
     <row r="13" spans="1:109" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="26">
+      <c r="D13" s="25">
         <v>15</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="25">
         <v>8</v>
       </c>
-      <c r="F13" s="26">
-        <v>15</v>
-      </c>
-      <c r="G13" s="26">
+      <c r="F13" s="25">
+        <v>18</v>
+      </c>
+      <c r="G13" s="25">
         <v>1</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H13" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:109" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="26">
-        <v>16</v>
-      </c>
-      <c r="E14" s="26">
-        <v>9</v>
-      </c>
-      <c r="F14" s="26">
-        <v>16</v>
-      </c>
-      <c r="G14" s="26">
-        <v>1</v>
-      </c>
-      <c r="H14" s="27">
-        <v>0</v>
+      <c r="D14" s="25">
+        <v>13</v>
+      </c>
+      <c r="E14" s="25">
+        <v>12</v>
+      </c>
+      <c r="F14" s="25">
+        <v>13</v>
+      </c>
+      <c r="G14" s="25">
+        <v>12</v>
+      </c>
+      <c r="H14" s="26">
+        <v>0.7</v>
       </c>
     </row>
     <row r="15" spans="1:109" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="26">
-        <v>24</v>
-      </c>
-      <c r="E15" s="26">
-        <v>8</v>
-      </c>
-      <c r="F15" s="26">
-        <v>24</v>
-      </c>
-      <c r="G15" s="26">
-        <v>1</v>
-      </c>
-      <c r="H15" s="27">
-        <v>0</v>
+      <c r="D15" s="25">
+        <v>13</v>
+      </c>
+      <c r="E15" s="25">
+        <v>18</v>
+      </c>
+      <c r="F15" s="25">
+        <v>13</v>
+      </c>
+      <c r="G15" s="25">
+        <v>12</v>
+      </c>
+      <c r="H15" s="26">
+        <v>0.9</v>
       </c>
     </row>
     <row r="16" spans="1:109" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="8"/>
-      <c r="D16" s="26">
-        <v>16</v>
-      </c>
-      <c r="E16" s="26">
-        <v>16</v>
-      </c>
-      <c r="F16" s="26">
-        <v>16</v>
-      </c>
-      <c r="G16" s="26">
-        <v>1</v>
-      </c>
-      <c r="H16" s="27">
-        <v>0</v>
+      <c r="D16" s="25">
+        <v>14</v>
+      </c>
+      <c r="E16" s="25">
+        <v>18</v>
+      </c>
+      <c r="F16" s="25">
+        <v>14</v>
+      </c>
+      <c r="G16" s="25">
+        <v>18</v>
+      </c>
+      <c r="H16" s="26">
+        <v>0.3</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="28">
+      <c r="D17" s="27">
         <v>31</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="25">
         <v>3</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="25">
         <v>31</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="25">
         <v>1</v>
       </c>
-      <c r="H17" s="27">
+      <c r="H17" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="22" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="8"/>
-      <c r="D18" s="26">
+      <c r="D18" s="25">
         <v>31</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="25">
         <v>6</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="25">
         <v>31</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="25">
         <v>1</v>
       </c>
-      <c r="H18" s="27">
+      <c r="H18" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="26">
+      <c r="D19" s="25">
         <v>36</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="25">
         <v>5</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="25">
         <v>36</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="25">
         <v>1</v>
       </c>
-      <c r="H19" s="27">
+      <c r="H19" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="22" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="26">
+      <c r="D20" s="25">
         <v>37</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="25">
         <v>7</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="25">
         <v>37</v>
       </c>
-      <c r="G20" s="26">
+      <c r="G20" s="25">
         <v>1</v>
       </c>
-      <c r="H20" s="27">
+      <c r="H20" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="26">
+      <c r="D21" s="25">
         <v>40</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="25">
         <v>8</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="25">
         <v>40</v>
       </c>
-      <c r="G21" s="26">
+      <c r="G21" s="25">
         <v>1</v>
       </c>
-      <c r="H21" s="27">
+      <c r="H21" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C22" s="8"/>
-      <c r="D22" s="26">
+      <c r="D22" s="25">
         <v>40</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="25">
         <v>11</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="25">
         <v>40</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G22" s="25">
         <v>1</v>
       </c>
-      <c r="H22" s="27">
+      <c r="H22" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="26">
+      <c r="D23" s="25">
         <v>43</v>
       </c>
-      <c r="E23" s="26">
+      <c r="E23" s="25">
         <v>10</v>
       </c>
-      <c r="F23" s="26">
+      <c r="F23" s="25">
         <v>43</v>
       </c>
-      <c r="G23" s="26">
+      <c r="G23" s="25">
         <v>1</v>
       </c>
-      <c r="H23" s="27">
+      <c r="H23" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="8"/>
-      <c r="D24" s="26">
+      <c r="D24" s="25">
         <v>36</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="25">
         <v>19</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="25">
         <v>36</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="25">
         <v>1</v>
       </c>
-      <c r="H24" s="27">
+      <c r="H24" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="26">
+      <c r="D25" s="25">
         <v>52</v>
       </c>
-      <c r="E25" s="26">
+      <c r="E25" s="25">
         <v>6</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="25">
         <v>52</v>
       </c>
-      <c r="G25" s="26">
+      <c r="G25" s="25">
         <v>1</v>
       </c>
-      <c r="H25" s="27">
+      <c r="H25" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="22" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="26">
+      <c r="D26" s="25">
         <v>57</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="25">
         <v>8</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="25">
         <v>57</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="25">
         <v>1</v>
       </c>
-      <c r="H26" s="27">
+      <c r="H26" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="22" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="26">
+      <c r="D27" s="25">
         <v>59</v>
       </c>
-      <c r="E27" s="26">
+      <c r="E27" s="25">
         <v>10</v>
       </c>
-      <c r="F27" s="26">
+      <c r="F27" s="25">
         <v>59</v>
       </c>
-      <c r="G27" s="26">
+      <c r="G27" s="25">
         <v>1</v>
       </c>
-      <c r="H27" s="27">
+      <c r="H27" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="22" t="s">
         <v>32</v>
       </c>
       <c r="C28" s="8"/>
-      <c r="D28" s="26">
+      <c r="D28" s="25">
         <v>64</v>
       </c>
-      <c r="E28" s="26">
+      <c r="E28" s="25">
         <v>10</v>
       </c>
-      <c r="F28" s="26">
+      <c r="F28" s="25">
         <v>64</v>
       </c>
-      <c r="G28" s="26">
+      <c r="G28" s="25">
         <v>1</v>
       </c>
-      <c r="H28" s="27">
+      <c r="H28" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="22" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="8"/>
-      <c r="D29" s="26">
+      <c r="D29" s="25">
         <v>71</v>
       </c>
-      <c r="E29" s="26">
+      <c r="E29" s="25">
         <v>8</v>
       </c>
-      <c r="F29" s="26">
+      <c r="F29" s="25">
         <v>71</v>
       </c>
-      <c r="G29" s="26">
+      <c r="G29" s="25">
         <v>1</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H29" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="22" t="s">
         <v>34</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="26">
+      <c r="D30" s="25">
         <v>83</v>
       </c>
-      <c r="E30" s="26">
+      <c r="E30" s="25">
         <v>10</v>
       </c>
-      <c r="F30" s="26">
+      <c r="F30" s="25">
         <v>83</v>
       </c>
-      <c r="G30" s="26">
+      <c r="G30" s="25">
         <v>1</v>
       </c>
-      <c r="H30" s="27">
+      <c r="H30" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="22" t="s">
         <v>35</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="26">
+      <c r="D31" s="25">
         <v>84</v>
       </c>
-      <c r="E31" s="26">
+      <c r="E31" s="25">
         <v>9</v>
       </c>
-      <c r="F31" s="26">
+      <c r="F31" s="25">
         <v>84</v>
       </c>
-      <c r="G31" s="26">
+      <c r="G31" s="25">
         <v>1</v>
       </c>
-      <c r="H31" s="27">
+      <c r="H31" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="8"/>
-      <c r="D32" s="26">
+      <c r="D32" s="25">
         <v>84</v>
       </c>
-      <c r="E32" s="26">
+      <c r="E32" s="25">
         <v>9</v>
       </c>
-      <c r="F32" s="26">
+      <c r="F32" s="25">
         <v>84</v>
       </c>
-      <c r="G32" s="26">
+      <c r="G32" s="25">
         <v>1</v>
       </c>
-      <c r="H32" s="27">
+      <c r="H32" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="26">
+      <c r="D33" s="25">
         <v>84</v>
       </c>
-      <c r="E33" s="26">
+      <c r="E33" s="25">
         <v>21</v>
       </c>
-      <c r="F33" s="26">
+      <c r="F33" s="25">
         <v>84</v>
       </c>
-      <c r="G33" s="26">
+      <c r="G33" s="25">
         <v>1</v>
       </c>
-      <c r="H33" s="27">
+      <c r="H33" s="26">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Gannt to 11-10-2014
</commit_message>
<xml_diff>
--- a/Fieldroid_Gantt.xlsx
+++ b/Fieldroid_Gantt.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t>Plan</t>
   </si>
@@ -287,6 +287,15 @@
   </si>
   <si>
     <t>Paint Full Scale Field w/ UI</t>
+  </si>
+  <si>
+    <t>Motion Planning Software</t>
+  </si>
+  <si>
+    <t>PID/Encoder Motor Integration</t>
+  </si>
+  <si>
+    <t>Mount All Parts</t>
   </si>
 </sst>
 </file>
@@ -1648,7 +1657,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="43"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="50"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1930,12 +1939,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DT34"/>
+  <dimension ref="A1:DT37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="9" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <pane xSplit="9" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="G28" sqref="G28"/>
+      <selection pane="topRight" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2000,7 +2009,7 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="22">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="P2" s="7"/>
       <c r="R2" s="8"/>
@@ -3045,7 +3054,7 @@
       </c>
       <c r="I16" s="68"/>
     </row>
-    <row r="17" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="69" t="s">
         <v>44</v>
       </c>
@@ -3067,7 +3076,7 @@
       </c>
       <c r="I17" s="73"/>
     </row>
-    <row r="18" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="74" t="s">
         <v>45</v>
       </c>
@@ -3085,11 +3094,11 @@
         <v>20</v>
       </c>
       <c r="H18" s="77">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I18" s="78"/>
     </row>
-    <row r="19" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="74" t="s">
         <v>16</v>
       </c>
@@ -3111,7 +3120,7 @@
       </c>
       <c r="I19" s="78"/>
     </row>
-    <row r="20" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="74" t="s">
         <v>48</v>
       </c>
@@ -3129,11 +3138,11 @@
         <v>32</v>
       </c>
       <c r="H20" s="77">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I20" s="78"/>
     </row>
-    <row r="21" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="80" t="s">
         <v>50</v>
       </c>
@@ -3151,11 +3160,11 @@
         <v>34</v>
       </c>
       <c r="H21" s="83">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I21" s="84"/>
     </row>
-    <row r="22" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="85" t="s">
         <v>17</v>
       </c>
@@ -3170,266 +3179,332 @@
         <v>31</v>
       </c>
       <c r="G22" s="87">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H22" s="88">
         <v>0.6</v>
       </c>
       <c r="I22" s="89"/>
     </row>
-    <row r="23" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="90" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="C23" s="91"/>
       <c r="D23" s="92">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E23" s="92">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F23" s="92">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G23" s="92">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H23" s="93">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="I23" s="94"/>
     </row>
-    <row r="24" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="90" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="91"/>
       <c r="D24" s="92">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="92">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F24" s="92">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G24" s="92">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H24" s="93">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="I24" s="94"/>
     </row>
-    <row r="25" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="90" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="91"/>
       <c r="D25" s="92">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E25" s="92">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F25" s="92">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G25" s="92">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H25" s="93">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I25" s="94"/>
     </row>
-    <row r="26" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="95" t="s">
+    <row r="26" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="90" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="91"/>
+      <c r="D26" s="92">
+        <v>40</v>
+      </c>
+      <c r="E26" s="92">
+        <v>15</v>
+      </c>
+      <c r="F26" s="92">
+        <v>40</v>
+      </c>
+      <c r="G26" s="92">
+        <v>16</v>
+      </c>
+      <c r="H26" s="93">
+        <v>0.1</v>
+      </c>
+      <c r="I26" s="94"/>
+    </row>
+    <row r="27" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="96"/>
-      <c r="D26" s="97">
+      <c r="C27" s="96"/>
+      <c r="D27" s="97">
         <v>43</v>
       </c>
-      <c r="E26" s="97">
+      <c r="E27" s="97">
         <v>21</v>
       </c>
-      <c r="F26" s="97">
+      <c r="F27" s="97">
         <v>43</v>
       </c>
-      <c r="G26" s="97">
+      <c r="G27" s="97">
         <v>21</v>
       </c>
-      <c r="H26" s="98">
+      <c r="H27" s="98">
         <v>0.2</v>
       </c>
-      <c r="I26" s="99"/>
+      <c r="I27" s="99"/>
     </row>
-    <row r="27" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="102" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="103"/>
-      <c r="D27" s="104">
-        <v>43</v>
-      </c>
-      <c r="E27" s="104">
-        <v>15</v>
-      </c>
-      <c r="F27" s="104">
-        <v>43</v>
-      </c>
-      <c r="G27" s="104">
-        <v>15</v>
-      </c>
-      <c r="H27" s="105">
-        <v>0</v>
-      </c>
-      <c r="I27" s="106"/>
-    </row>
-    <row r="28" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="102" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C28" s="103"/>
       <c r="D28" s="104">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E28" s="104">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F28" s="104">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G28" s="104">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H28" s="105">
         <v>0</v>
       </c>
       <c r="I28" s="106"/>
     </row>
-    <row r="29" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="107" t="s">
+    <row r="29" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="102" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="103"/>
+      <c r="D29" s="104">
+        <v>34</v>
+      </c>
+      <c r="E29" s="104">
+        <v>23</v>
+      </c>
+      <c r="F29" s="104">
+        <v>34</v>
+      </c>
+      <c r="G29" s="104">
+        <v>23</v>
+      </c>
+      <c r="H29" s="105">
+        <v>0.7</v>
+      </c>
+      <c r="I29" s="106"/>
+    </row>
+    <row r="30" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="102" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="103"/>
+      <c r="D30" s="104">
+        <v>43</v>
+      </c>
+      <c r="E30" s="104">
+        <v>15</v>
+      </c>
+      <c r="F30" s="104">
+        <v>43</v>
+      </c>
+      <c r="G30" s="104">
+        <v>15</v>
+      </c>
+      <c r="H30" s="105">
+        <v>0.4</v>
+      </c>
+      <c r="I30" s="106"/>
+    </row>
+    <row r="31" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="102" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="103"/>
+      <c r="D31" s="104">
+        <v>59</v>
+      </c>
+      <c r="E31" s="104">
+        <v>6</v>
+      </c>
+      <c r="F31" s="104">
+        <v>59</v>
+      </c>
+      <c r="G31" s="104">
+        <v>6</v>
+      </c>
+      <c r="H31" s="105">
+        <v>0.4</v>
+      </c>
+      <c r="I31" s="106"/>
+    </row>
+    <row r="32" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="108"/>
-      <c r="D29" s="109">
+      <c r="C32" s="108"/>
+      <c r="D32" s="109">
         <v>83</v>
       </c>
-      <c r="E29" s="109">
+      <c r="E32" s="109">
         <v>10</v>
       </c>
-      <c r="F29" s="109">
+      <c r="F32" s="109">
         <v>83</v>
       </c>
-      <c r="G29" s="109">
+      <c r="G32" s="109">
         <v>1</v>
       </c>
-      <c r="H29" s="110">
+      <c r="H32" s="110">
         <v>0</v>
       </c>
-      <c r="I29" s="111"/>
-    </row>
-    <row r="30" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="112" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="113"/>
-      <c r="D30" s="114">
-        <v>84</v>
-      </c>
-      <c r="E30" s="114">
-        <v>18</v>
-      </c>
-      <c r="F30" s="114">
-        <v>84</v>
-      </c>
-      <c r="G30" s="114">
-        <v>1</v>
-      </c>
-      <c r="H30" s="115">
-        <v>0</v>
-      </c>
-      <c r="I30" s="116"/>
-    </row>
-    <row r="31" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="112" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="113"/>
-      <c r="D31" s="114">
-        <v>84</v>
-      </c>
-      <c r="E31" s="114">
-        <v>9</v>
-      </c>
-      <c r="F31" s="114">
-        <v>84</v>
-      </c>
-      <c r="G31" s="114">
-        <v>1</v>
-      </c>
-      <c r="H31" s="115">
-        <v>0</v>
-      </c>
-      <c r="I31" s="116"/>
-    </row>
-    <row r="32" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="117" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="118"/>
-      <c r="D32" s="114">
-        <v>84</v>
-      </c>
-      <c r="E32" s="114">
-        <v>18</v>
-      </c>
-      <c r="F32" s="114">
-        <v>84</v>
-      </c>
-      <c r="G32" s="114">
-        <v>1</v>
-      </c>
-      <c r="H32" s="115">
-        <v>0</v>
-      </c>
-      <c r="I32" s="116"/>
-      <c r="DF32" s="100"/>
+      <c r="I32" s="111"/>
     </row>
     <row r="33" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="119" t="s">
+      <c r="B33" s="112" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="113"/>
+      <c r="D33" s="114">
+        <v>84</v>
+      </c>
+      <c r="E33" s="114">
+        <v>18</v>
+      </c>
+      <c r="F33" s="114">
+        <v>84</v>
+      </c>
+      <c r="G33" s="114">
+        <v>1</v>
+      </c>
+      <c r="H33" s="115">
+        <v>0</v>
+      </c>
+      <c r="I33" s="116"/>
+    </row>
+    <row r="34" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="112" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="113"/>
+      <c r="D34" s="114">
+        <v>84</v>
+      </c>
+      <c r="E34" s="114">
+        <v>9</v>
+      </c>
+      <c r="F34" s="114">
+        <v>84</v>
+      </c>
+      <c r="G34" s="114">
+        <v>1</v>
+      </c>
+      <c r="H34" s="115">
+        <v>0</v>
+      </c>
+      <c r="I34" s="116"/>
+    </row>
+    <row r="35" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="117" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="118"/>
+      <c r="D35" s="114">
+        <v>84</v>
+      </c>
+      <c r="E35" s="114">
+        <v>18</v>
+      </c>
+      <c r="F35" s="114">
+        <v>84</v>
+      </c>
+      <c r="G35" s="114">
+        <v>1</v>
+      </c>
+      <c r="H35" s="115">
+        <v>0</v>
+      </c>
+      <c r="I35" s="116"/>
+      <c r="DF35" s="100"/>
+    </row>
+    <row r="36" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="120"/>
-      <c r="D33" s="121">
+      <c r="C36" s="120"/>
+      <c r="D36" s="121">
         <v>84</v>
       </c>
-      <c r="E33" s="121">
+      <c r="E36" s="121">
         <v>18</v>
       </c>
-      <c r="F33" s="121">
+      <c r="F36" s="121">
         <v>84</v>
       </c>
-      <c r="G33" s="121">
+      <c r="G36" s="121">
         <v>1</v>
       </c>
-      <c r="H33" s="122">
+      <c r="H36" s="122">
         <v>0</v>
       </c>
-      <c r="I33" s="123"/>
-      <c r="DF33" s="100"/>
+      <c r="I36" s="123"/>
+      <c r="DF36" s="100"/>
     </row>
-    <row r="34" spans="2:110" x14ac:dyDescent="0.3">
-      <c r="DF34" s="101"/>
+    <row r="37" spans="2:110" x14ac:dyDescent="0.3">
+      <c r="DF37" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
-  <conditionalFormatting sqref="DP33:DT33 J33:DL33 J6:DT31">
+  <conditionalFormatting sqref="DP36:DT36 J36:DL36 J6:DT34">
     <cfRule type="expression" dxfId="33" priority="172">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3455,7 +3530,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B34:DE34">
+  <conditionalFormatting sqref="B37:DE37">
     <cfRule type="expression" dxfId="25" priority="173">
       <formula>TRUE</formula>
     </cfRule>
@@ -3465,7 +3540,7 @@
       <formula>J$5=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DM33:DO33">
+  <conditionalFormatting sqref="DM36:DO36">
     <cfRule type="expression" dxfId="23" priority="26">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3491,7 +3566,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DP32:DT32 J32:DL32">
+  <conditionalFormatting sqref="DP35:DT35 J35:DL35">
     <cfRule type="expression" dxfId="15" priority="9">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3517,7 +3592,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DM32:DO32">
+  <conditionalFormatting sqref="DM35:DO35">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated the Gantt Chart with controls additions
</commit_message>
<xml_diff>
--- a/Fieldroid_Gantt.xlsx
+++ b/Fieldroid_Gantt.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="126">
   <si>
     <t>Plan</t>
   </si>
@@ -400,9 +400,6 @@
     <t>Derivative Control</t>
   </si>
   <si>
-    <t>Wobbly Bug Removal</t>
-  </si>
-  <si>
     <t>Submit Last PCB Design</t>
   </si>
   <si>
@@ -461,6 +458,36 @@
   </si>
   <si>
     <t>Case Design Iteration 2 and Printed</t>
+  </si>
+  <si>
+    <t>Meet with Nathan</t>
+  </si>
+  <si>
+    <t>Serial Comm w/ Code</t>
+  </si>
+  <si>
+    <t>Fix Motor Controller</t>
+  </si>
+  <si>
+    <t>Closed Loop on Blocks</t>
+  </si>
+  <si>
+    <t>MJT - Straight Line</t>
+  </si>
+  <si>
+    <t>MJT - Curves</t>
+  </si>
+  <si>
+    <t>Cleaning Code</t>
+  </si>
+  <si>
+    <t>Connected Points - Quadratic Progr.</t>
+  </si>
+  <si>
+    <t>Localization Kinematic Transformation</t>
+  </si>
+  <si>
+    <t>Code Integration (new control)</t>
   </si>
 </sst>
 </file>
@@ -2321,7 +2348,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="11"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2659,18 +2686,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DT33"/>
+  <dimension ref="A1:DT42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="9" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <pane xSplit="9" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="AB19" sqref="AB19"/>
+      <selection pane="topRight" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="26.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.25" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.75" style="1" bestFit="1" customWidth="1"/>
@@ -2718,7 +2745,7 @@
         <v>75</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I2" s="27"/>
       <c r="J2" s="120" t="s">
@@ -2729,7 +2756,7 @@
       <c r="M2" s="121"/>
       <c r="N2" s="121"/>
       <c r="O2" s="122">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="P2" s="121"/>
       <c r="R2" s="123"/>
@@ -3770,7 +3797,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="40">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I6" s="41"/>
     </row>
@@ -3794,13 +3821,13 @@
         <v>8</v>
       </c>
       <c r="H7" s="43">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I7" s="44"/>
     </row>
     <row r="8" spans="1:124" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="107" t="s">
         <v>84</v>
@@ -3818,7 +3845,7 @@
         <v>19</v>
       </c>
       <c r="H8" s="43">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I8" s="44"/>
     </row>
@@ -3842,7 +3869,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="44"/>
     </row>
@@ -3866,7 +3893,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="44"/>
     </row>
@@ -3890,7 +3917,7 @@
         <v>15</v>
       </c>
       <c r="H11" s="43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="44"/>
     </row>
@@ -3944,470 +3971,686 @@
     </row>
     <row r="14" spans="1:124" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="55" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="C14" s="109" t="s">
         <v>88</v>
       </c>
       <c r="D14" s="47">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E14" s="47">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F14" s="47">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G14" s="47">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H14" s="48">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I14" s="56"/>
     </row>
     <row r="15" spans="1:124" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="55" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="C15" s="109" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D15" s="47">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E15" s="47">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F15" s="47">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G15" s="47">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="H15" s="48">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:124" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="55" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="C16" s="109" t="s">
         <v>85</v>
       </c>
       <c r="D16" s="47">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E16" s="47">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F16" s="47">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="G16" s="47">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H16" s="48">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I16" s="56"/>
     </row>
-    <row r="17" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="55" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C17" s="109" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17" s="47">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E17" s="47">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F17" s="47">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G17" s="47">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="H17" s="48">
         <v>0</v>
       </c>
       <c r="I17" s="56"/>
     </row>
-    <row r="18" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="57" t="s">
+    <row r="18" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="47">
+        <v>25</v>
+      </c>
+      <c r="E18" s="47">
+        <v>9</v>
+      </c>
+      <c r="F18" s="47">
+        <v>25</v>
+      </c>
+      <c r="G18" s="47">
+        <v>9</v>
+      </c>
+      <c r="H18" s="48">
+        <v>0</v>
+      </c>
+      <c r="I18" s="56"/>
+    </row>
+    <row r="19" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="109" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="47">
+        <v>17</v>
+      </c>
+      <c r="E19" s="47">
+        <v>7</v>
+      </c>
+      <c r="F19" s="47">
+        <v>17</v>
+      </c>
+      <c r="G19" s="47">
+        <v>7</v>
+      </c>
+      <c r="H19" s="48">
+        <v>0</v>
+      </c>
+      <c r="I19" s="56"/>
+    </row>
+    <row r="20" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="109" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="47">
+        <v>11</v>
+      </c>
+      <c r="E20" s="47">
+        <v>16</v>
+      </c>
+      <c r="F20" s="47">
+        <v>11</v>
+      </c>
+      <c r="G20" s="47">
+        <v>16</v>
+      </c>
+      <c r="H20" s="48">
+        <v>0</v>
+      </c>
+      <c r="I20" s="56"/>
+    </row>
+    <row r="21" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="109" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="47">
+        <v>20</v>
+      </c>
+      <c r="E21" s="47">
+        <v>14</v>
+      </c>
+      <c r="F21" s="47">
+        <v>20</v>
+      </c>
+      <c r="G21" s="47">
+        <v>14</v>
+      </c>
+      <c r="H21" s="48">
+        <v>0</v>
+      </c>
+      <c r="I21" s="56"/>
+    </row>
+    <row r="22" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="109" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="47">
+        <v>11</v>
+      </c>
+      <c r="E22" s="47">
+        <v>23</v>
+      </c>
+      <c r="F22" s="47">
+        <v>11</v>
+      </c>
+      <c r="G22" s="47">
+        <v>23</v>
+      </c>
+      <c r="H22" s="48">
+        <v>0</v>
+      </c>
+      <c r="I22" s="56"/>
+    </row>
+    <row r="23" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="47">
+        <v>20</v>
+      </c>
+      <c r="E23" s="47">
+        <v>9</v>
+      </c>
+      <c r="F23" s="47">
+        <v>20</v>
+      </c>
+      <c r="G23" s="47">
+        <v>9</v>
+      </c>
+      <c r="H23" s="48">
+        <v>0</v>
+      </c>
+      <c r="I23" s="56"/>
+    </row>
+    <row r="24" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="110" t="s">
+      <c r="C24" s="110" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D24" s="58">
         <v>11</v>
       </c>
-      <c r="E18" s="59">
+      <c r="E24" s="59">
         <v>23</v>
       </c>
-      <c r="F18" s="59">
+      <c r="F24" s="59">
         <v>11</v>
       </c>
-      <c r="G18" s="59">
+      <c r="G24" s="59">
         <v>23</v>
       </c>
-      <c r="H18" s="60">
+      <c r="H24" s="60">
         <v>0</v>
       </c>
-      <c r="I18" s="61"/>
-    </row>
-    <row r="19" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="62" t="s">
+      <c r="I24" s="61"/>
+    </row>
+    <row r="25" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="111" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="63">
+        <v>5</v>
+      </c>
+      <c r="E25" s="63">
+        <v>43</v>
+      </c>
+      <c r="F25" s="63">
+        <v>5</v>
+      </c>
+      <c r="G25" s="63">
+        <v>43</v>
+      </c>
+      <c r="H25" s="68">
+        <v>0</v>
+      </c>
+      <c r="I25" s="65"/>
+    </row>
+    <row r="26" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="112" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="67">
+        <v>30</v>
+      </c>
+      <c r="E26" s="67">
+        <v>18</v>
+      </c>
+      <c r="F26" s="67">
+        <v>30</v>
+      </c>
+      <c r="G26" s="67">
+        <v>18</v>
+      </c>
+      <c r="H26" s="68">
+        <v>0</v>
+      </c>
+      <c r="I26" s="69"/>
+    </row>
+    <row r="27" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="112" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="67">
+        <v>26</v>
+      </c>
+      <c r="E27" s="67">
+        <v>22</v>
+      </c>
+      <c r="F27" s="67">
+        <v>26</v>
+      </c>
+      <c r="G27" s="67">
+        <v>22</v>
+      </c>
+      <c r="H27" s="68">
+        <v>0</v>
+      </c>
+      <c r="I27" s="69"/>
+    </row>
+    <row r="28" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="112" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="67">
+        <v>26</v>
+      </c>
+      <c r="E28" s="67">
+        <v>22</v>
+      </c>
+      <c r="F28" s="67">
+        <v>26</v>
+      </c>
+      <c r="G28" s="67">
+        <v>22</v>
+      </c>
+      <c r="H28" s="68">
+        <v>0</v>
+      </c>
+      <c r="I28" s="69"/>
+    </row>
+    <row r="29" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="112" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="67">
+        <v>34</v>
+      </c>
+      <c r="E29" s="67">
+        <v>14</v>
+      </c>
+      <c r="F29" s="67">
+        <v>34</v>
+      </c>
+      <c r="G29" s="67">
+        <v>14</v>
+      </c>
+      <c r="H29" s="68">
+        <v>0</v>
+      </c>
+      <c r="I29" s="69"/>
+    </row>
+    <row r="30" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="66" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="112" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="67">
+        <v>34</v>
+      </c>
+      <c r="E30" s="67">
+        <v>14</v>
+      </c>
+      <c r="F30" s="67">
+        <v>34</v>
+      </c>
+      <c r="G30" s="67">
+        <v>14</v>
+      </c>
+      <c r="H30" s="68">
+        <v>0</v>
+      </c>
+      <c r="I30" s="69"/>
+    </row>
+    <row r="31" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="112" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="70">
+        <v>10</v>
+      </c>
+      <c r="E31" s="67">
+        <v>33</v>
+      </c>
+      <c r="F31" s="67">
+        <v>10</v>
+      </c>
+      <c r="G31" s="67">
+        <v>33</v>
+      </c>
+      <c r="H31" s="68">
+        <v>0</v>
+      </c>
+      <c r="I31" s="69"/>
+    </row>
+    <row r="32" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="113" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="72">
+        <v>8</v>
+      </c>
+      <c r="E32" s="72">
+        <v>35</v>
+      </c>
+      <c r="F32" s="72">
+        <v>8</v>
+      </c>
+      <c r="G32" s="72">
+        <v>35</v>
+      </c>
+      <c r="H32" s="73">
+        <v>0</v>
+      </c>
+      <c r="I32" s="74"/>
+    </row>
+    <row r="33" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="114" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="76">
+        <v>34</v>
+      </c>
+      <c r="E33" s="76">
+        <v>19</v>
+      </c>
+      <c r="F33" s="76">
+        <v>34</v>
+      </c>
+      <c r="G33" s="76">
+        <v>19</v>
+      </c>
+      <c r="H33" s="77">
+        <v>0</v>
+      </c>
+      <c r="I33" s="78"/>
+    </row>
+    <row r="34" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="111" t="s">
+      <c r="C34" s="115" t="s">
         <v>84</v>
       </c>
-      <c r="D19" s="63">
-        <v>5</v>
-      </c>
-      <c r="E19" s="63">
-        <v>43</v>
-      </c>
-      <c r="F19" s="63">
-        <v>5</v>
-      </c>
-      <c r="G19" s="63">
-        <v>43</v>
-      </c>
-      <c r="H19" s="68">
+      <c r="D34" s="80">
+        <v>40</v>
+      </c>
+      <c r="E34" s="80">
+        <v>14</v>
+      </c>
+      <c r="F34" s="80">
+        <v>40</v>
+      </c>
+      <c r="G34" s="80">
+        <v>14</v>
+      </c>
+      <c r="H34" s="81">
         <v>0</v>
       </c>
-      <c r="I19" s="65"/>
-    </row>
-    <row r="20" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="66" t="s">
+      <c r="I34" s="82"/>
+    </row>
+    <row r="35" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="79" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="80">
+        <v>34</v>
+      </c>
+      <c r="E35" s="80">
+        <v>16</v>
+      </c>
+      <c r="F35" s="80">
+        <v>34</v>
+      </c>
+      <c r="G35" s="80">
+        <v>16</v>
+      </c>
+      <c r="H35" s="81">
+        <v>0</v>
+      </c>
+      <c r="I35" s="82"/>
+    </row>
+    <row r="36" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="79" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="115" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" s="80">
+        <v>40</v>
+      </c>
+      <c r="E36" s="80">
+        <v>14</v>
+      </c>
+      <c r="F36" s="80">
+        <v>40</v>
+      </c>
+      <c r="G36" s="80">
+        <v>14</v>
+      </c>
+      <c r="H36" s="186">
+        <v>0</v>
+      </c>
+      <c r="I36" s="82"/>
+    </row>
+    <row r="37" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="83" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="112" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="67">
-        <v>30</v>
-      </c>
-      <c r="E20" s="67">
-        <v>18</v>
-      </c>
-      <c r="F20" s="67">
-        <v>30</v>
-      </c>
-      <c r="G20" s="67">
-        <v>18</v>
-      </c>
-      <c r="H20" s="68">
+      <c r="C37" s="116" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="84">
+        <v>40</v>
+      </c>
+      <c r="E37" s="84">
+        <v>29</v>
+      </c>
+      <c r="F37" s="84">
+        <v>40</v>
+      </c>
+      <c r="G37" s="84">
+        <v>29</v>
+      </c>
+      <c r="H37" s="85">
         <v>0</v>
       </c>
-      <c r="I20" s="69"/>
-    </row>
-    <row r="21" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="66" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="112" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="67">
+      <c r="I37" s="86"/>
+    </row>
+    <row r="38" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="89" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="117" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="90">
+        <v>48</v>
+      </c>
+      <c r="E38" s="90">
+        <v>21</v>
+      </c>
+      <c r="F38" s="90">
+        <v>48</v>
+      </c>
+      <c r="G38" s="90">
+        <v>21</v>
+      </c>
+      <c r="H38" s="91">
+        <v>0</v>
+      </c>
+      <c r="I38" s="92"/>
+    </row>
+    <row r="39" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="89" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="117" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="90">
+        <v>54</v>
+      </c>
+      <c r="E39" s="90">
+        <v>12</v>
+      </c>
+      <c r="F39" s="90">
+        <v>54</v>
+      </c>
+      <c r="G39" s="90">
+        <v>12</v>
+      </c>
+      <c r="H39" s="196">
+        <v>0</v>
+      </c>
+      <c r="I39" s="92"/>
+    </row>
+    <row r="40" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="93" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="118" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="94">
+        <v>69</v>
+      </c>
+      <c r="E40" s="94">
         <v>26</v>
       </c>
-      <c r="E21" s="67">
-        <v>22</v>
-      </c>
-      <c r="F21" s="67">
+      <c r="F40" s="94">
+        <v>69</v>
+      </c>
+      <c r="G40" s="94">
         <v>26</v>
       </c>
-      <c r="G21" s="67">
-        <v>22</v>
-      </c>
-      <c r="H21" s="68">
+      <c r="H40" s="197">
         <v>0</v>
       </c>
-      <c r="I21" s="69"/>
-    </row>
-    <row r="22" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="66" t="s">
-        <v>102</v>
-      </c>
-      <c r="C22" s="112" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="67">
-        <v>26</v>
-      </c>
-      <c r="E22" s="67">
-        <v>22</v>
-      </c>
-      <c r="F22" s="67">
-        <v>26</v>
-      </c>
-      <c r="G22" s="67">
-        <v>22</v>
-      </c>
-      <c r="H22" s="68">
+      <c r="I40" s="96"/>
+    </row>
+    <row r="41" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="101" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="119" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="102">
+        <v>95</v>
+      </c>
+      <c r="E41" s="102">
+        <v>9</v>
+      </c>
+      <c r="F41" s="102">
+        <v>95</v>
+      </c>
+      <c r="G41" s="102">
+        <v>9</v>
+      </c>
+      <c r="H41" s="103">
         <v>0</v>
       </c>
-      <c r="I22" s="69"/>
-    </row>
-    <row r="23" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="112" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="70">
-        <v>10</v>
-      </c>
-      <c r="E23" s="67">
-        <v>33</v>
-      </c>
-      <c r="F23" s="67">
-        <v>10</v>
-      </c>
-      <c r="G23" s="67">
-        <v>33</v>
-      </c>
-      <c r="H23" s="68">
-        <v>0</v>
-      </c>
-      <c r="I23" s="69"/>
-    </row>
-    <row r="24" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="71" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24" s="113" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="72">
-        <v>8</v>
-      </c>
-      <c r="E24" s="72">
-        <v>35</v>
-      </c>
-      <c r="F24" s="72">
-        <v>8</v>
-      </c>
-      <c r="G24" s="72">
-        <v>35</v>
-      </c>
-      <c r="H24" s="73">
-        <v>0</v>
-      </c>
-      <c r="I24" s="74"/>
-    </row>
-    <row r="25" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="75" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" s="114" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="76">
-        <v>34</v>
-      </c>
-      <c r="E25" s="76">
-        <v>19</v>
-      </c>
-      <c r="F25" s="76">
-        <v>34</v>
-      </c>
-      <c r="G25" s="76">
-        <v>19</v>
-      </c>
-      <c r="H25" s="77">
-        <v>0</v>
-      </c>
-      <c r="I25" s="78"/>
-    </row>
-    <row r="26" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="79" t="s">
-        <v>116</v>
-      </c>
-      <c r="C26" s="115" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="80">
-        <v>40</v>
-      </c>
-      <c r="E26" s="80">
-        <v>14</v>
-      </c>
-      <c r="F26" s="80">
-        <v>40</v>
-      </c>
-      <c r="G26" s="80">
-        <v>14</v>
-      </c>
-      <c r="H26" s="81">
-        <v>0</v>
-      </c>
-      <c r="I26" s="82"/>
-    </row>
-    <row r="27" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="79" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" s="115" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="80">
-        <v>40</v>
-      </c>
-      <c r="E27" s="80">
-        <v>14</v>
-      </c>
-      <c r="F27" s="80">
-        <v>40</v>
-      </c>
-      <c r="G27" s="80">
-        <v>14</v>
-      </c>
-      <c r="H27" s="186">
-        <v>0</v>
-      </c>
-      <c r="I27" s="82"/>
-    </row>
-    <row r="28" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="83" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="116" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="84">
-        <v>40</v>
-      </c>
-      <c r="E28" s="84">
-        <v>29</v>
-      </c>
-      <c r="F28" s="84">
-        <v>40</v>
-      </c>
-      <c r="G28" s="84">
-        <v>29</v>
-      </c>
-      <c r="H28" s="85">
-        <v>0</v>
-      </c>
-      <c r="I28" s="86"/>
-    </row>
-    <row r="29" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="89" t="s">
-        <v>108</v>
-      </c>
-      <c r="C29" s="117" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="90">
-        <v>48</v>
-      </c>
-      <c r="E29" s="90">
-        <v>21</v>
-      </c>
-      <c r="F29" s="90">
-        <v>48</v>
-      </c>
-      <c r="G29" s="90">
-        <v>21</v>
-      </c>
-      <c r="H29" s="91">
-        <v>0</v>
-      </c>
-      <c r="I29" s="92"/>
-    </row>
-    <row r="30" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="89" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" s="117" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="90">
-        <v>54</v>
-      </c>
-      <c r="E30" s="90">
-        <v>12</v>
-      </c>
-      <c r="F30" s="90">
-        <v>54</v>
-      </c>
-      <c r="G30" s="90">
-        <v>12</v>
-      </c>
-      <c r="H30" s="196">
-        <v>0</v>
-      </c>
-      <c r="I30" s="92"/>
-    </row>
-    <row r="31" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="93" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" s="118" t="s">
-        <v>113</v>
-      </c>
-      <c r="D31" s="94">
-        <v>69</v>
-      </c>
-      <c r="E31" s="94">
-        <v>26</v>
-      </c>
-      <c r="F31" s="94">
-        <v>69</v>
-      </c>
-      <c r="G31" s="94">
-        <v>26</v>
-      </c>
-      <c r="H31" s="197">
-        <v>0</v>
-      </c>
-      <c r="I31" s="96"/>
-    </row>
-    <row r="32" spans="2:110" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="101" t="s">
-        <v>112</v>
-      </c>
-      <c r="C32" s="119" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="102">
-        <v>95</v>
-      </c>
-      <c r="E32" s="102">
-        <v>9</v>
-      </c>
-      <c r="F32" s="102">
-        <v>95</v>
-      </c>
-      <c r="G32" s="102">
-        <v>9</v>
-      </c>
-      <c r="H32" s="103">
-        <v>0</v>
-      </c>
-      <c r="I32" s="104"/>
-      <c r="DF32" s="87"/>
-    </row>
-    <row r="33" spans="110:110" x14ac:dyDescent="0.3">
-      <c r="DF33" s="88"/>
+      <c r="I41" s="104"/>
+      <c r="DF41" s="87"/>
+    </row>
+    <row r="42" spans="2:110" x14ac:dyDescent="0.3">
+      <c r="DF42" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="H5:I5"/>
   </mergeCells>
-  <conditionalFormatting sqref="DP32:DT32 J32:DL32 J6:DT31">
+  <conditionalFormatting sqref="DP41:DT41 J41:DL41 J6:DT40">
     <cfRule type="expression" dxfId="51" priority="25">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -4433,7 +4676,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33:DE33">
+  <conditionalFormatting sqref="B42:DE42">
     <cfRule type="expression" dxfId="43" priority="26">
       <formula>TRUE</formula>
     </cfRule>
@@ -4443,7 +4686,7 @@
       <formula>J$5=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DM32:DO32">
+  <conditionalFormatting sqref="DM41:DO41">
     <cfRule type="expression" dxfId="41" priority="17">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>